<commit_message>
Perfect run, choose excel to be input for add.
</commit_message>
<xml_diff>
--- a/For_Run/9_2_2023.xlsx
+++ b/For_Run/9_2_2023.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Keyword</t>
   </si>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>wool dryer balls made in usa</t>
-  </si>
-  <si>
-    <t>wool dryer balls</t>
   </si>
   <si>
     <t>kids hangers</t>
@@ -563,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -621,12 +615,12 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -662,16 +656,6 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -714,15 +698,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Category xmlns="e383b11b-17d9-441d-99cc-a70c92f2591c">Excel Templates</Category>
-    <Language xmlns="e383b11b-17d9-441d-99cc-a70c92f2591c">english</Language>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002241A8E177F93744B10679941878564E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a947d23e8ab797820983737d3f7a3e35">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e383b11b-17d9-441d-99cc-a70c92f2591c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9583d43e149d759549a4b55e875b7135" ns2:_="">
     <xsd:import namespace="e383b11b-17d9-441d-99cc-a70c92f2591c"/>
@@ -863,6 +838,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Category xmlns="e383b11b-17d9-441d-99cc-a70c92f2591c">Excel Templates</Category>
+    <Language xmlns="e383b11b-17d9-441d-99cc-a70c92f2591c">english</Language>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA1037B-2CEB-4278-8B9E-F31B75BCC278}">
   <ds:schemaRefs>
@@ -872,22 +856,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B11F3C-8D5A-4FE8-A577-D7AAB645DDDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="e383b11b-17d9-441d-99cc-a70c92f2591c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20FA202B-0B83-4D9C-9148-C6E3F9E153BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -903,4 +871,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B11F3C-8D5A-4FE8-A577-D7AAB645DDDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="e383b11b-17d9-441d-99cc-a70c92f2591c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>